<commit_message>
updated mouse weight sheets
</commit_message>
<xml_diff>
--- a/DATA/body_weights_measurement.xlsx
+++ b/DATA/body_weights_measurement.xlsx
@@ -5,23 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarudutt/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarudutt/Documents/impac-tb-r/CODING-TEAM-BOOKDOWN-/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8ED4F23-8099-0745-8700-2DE4010C55B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1157DD-D47B-D840-822C-14579A258830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16360" activeTab="5" xr2:uid="{EF754327-75C9-0D46-A1B0-E47C524B8CAE}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16360" activeTab="3" xr2:uid="{EF754327-75C9-0D46-A1B0-E47C524B8CAE}"/>
   </bookViews>
   <sheets>
     <sheet name="before_vaccination" sheetId="1" r:id="rId1"/>
     <sheet name="6.3.22" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId3"/>
-    <sheet name="6-9-22" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
-    <sheet name="6-16-22" sheetId="4" r:id="rId6"/>
-    <sheet name="6-21-22" sheetId="5" r:id="rId7"/>
-    <sheet name="7-1-22" sheetId="6" r:id="rId8"/>
-    <sheet name="07-07-22" sheetId="8" r:id="rId9"/>
+    <sheet name="6-9-22" sheetId="3" r:id="rId3"/>
+    <sheet name="6-16-22" sheetId="4" r:id="rId4"/>
+    <sheet name="6-21-22" sheetId="5" r:id="rId5"/>
+    <sheet name="7-1-22" sheetId="6" r:id="rId6"/>
+    <sheet name="07-07-22" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -10046,18 +10044,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5381CCEB-1147-4E14-89E0-7E14705A124F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DEDDE3-1394-49BF-B818-8D3D8D78518B}">
   <dimension ref="A1:K141"/>
   <sheetViews>
@@ -14766,19 +14752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD63F08F-FFC5-47FF-A93B-36D2B57ECBA6}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CEF4192-D164-4CF6-8C97-39E6CE474352}">
   <dimension ref="A1:K141"/>
   <sheetViews>
@@ -19460,7 +19434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E255660F-2462-47DD-A055-F25B5C708F02}">
   <dimension ref="A1:K141"/>
   <sheetViews>
@@ -24157,7 +24131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282F7039-F2FD-4D49-A7D4-099B758AE087}">
   <dimension ref="A1:K141"/>
   <sheetViews>
@@ -28870,7 +28844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57C79E-F215-4103-AD42-D55276101BC9}">
   <dimension ref="A1:K141"/>
   <sheetViews>
@@ -33570,6 +33544,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="03c6cdc5-a326-4596-8bb5-5a108e6a189f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdb376e-ba08-4f94-9941-9e68dfd9ed35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D29CD47150B3D44192901CB20E6ABB56" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1b439f2d7c6d7abf5415dab7afed1a4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9bdb376e-ba08-4f94-9941-9e68dfd9ed35" xmlns:ns3="03c6cdc5-a326-4596-8bb5-5a108e6a189f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3257b63d3648651b426df57415bcf4c4" ns2:_="" ns3:_="">
     <xsd:import namespace="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
@@ -33758,27 +33752,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="03c6cdc5-a326-4596-8bb5-5a108e6a189f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdb376e-ba08-4f94-9941-9e68dfd9ed35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F20E8B07-673B-45FB-9B52-2C6DE9B56665}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E36FD8F2-91D2-40E1-98F1-66460F47765C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="03c6cdc5-a326-4596-8bb5-5a108e6a189f"/>
+    <ds:schemaRef ds:uri="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937EA692-236A-4E27-A58D-20EAE7DF481C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33795,23 +33788,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E36FD8F2-91D2-40E1-98F1-66460F47765C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="03c6cdc5-a326-4596-8bb5-5a108e6a189f"/>
-    <ds:schemaRef ds:uri="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F20E8B07-673B-45FB-9B52-2C6DE9B56665}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add more on how to record mouse weights
</commit_message>
<xml_diff>
--- a/DATA/body_weights_measurement.xlsx
+++ b/DATA/body_weights_measurement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarudutt/Documents/impac-tb-r/CODING-TEAM-BOOKDOWN-/DATA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgianaanderson/Documents/my_books/CODING-TEAM-BOOKDOWN-/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1157DD-D47B-D840-822C-14579A258830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF46371-BFCB-4944-A9B4-B86F0D934848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16360" activeTab="3" xr2:uid="{EF754327-75C9-0D46-A1B0-E47C524B8CAE}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="16260" activeTab="6" xr2:uid="{EF754327-75C9-0D46-A1B0-E47C524B8CAE}"/>
   </bookViews>
   <sheets>
     <sheet name="before_vaccination" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6529" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6949" uniqueCount="72">
   <si>
     <t>who_collected</t>
   </si>
@@ -248,6 +248,15 @@
   </si>
   <si>
     <t>mouse 1 separated from the cage</t>
+  </si>
+  <si>
+    <t>"June 21, 2022"</t>
+  </si>
+  <si>
+    <t>"July 1, 2022"</t>
+  </si>
+  <si>
+    <t>"July 7, 2022"</t>
   </si>
 </sst>
 </file>
@@ -5378,7 +5387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C25201A-ED7D-4B98-B534-D23BB5ECFA5E}">
   <dimension ref="A1:K148"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -14756,8 +14765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CEF4192-D164-4CF6-8C97-39E6CE474352}">
   <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19439,7 +19448,7 @@
   <dimension ref="A1:K141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="A1:K141"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19494,8 +19503,8 @@
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="3">
-        <v>44733</v>
+      <c r="B2" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -19527,8 +19536,8 @@
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="3">
-        <v>44733</v>
+      <c r="B3" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -19560,8 +19569,8 @@
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="3">
-        <v>44733</v>
+      <c r="B4" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
@@ -19593,8 +19602,8 @@
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="3">
-        <v>44733</v>
+      <c r="B5" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
@@ -19626,8 +19635,8 @@
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="3">
-        <v>44733</v>
+      <c r="B6" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
@@ -19659,8 +19668,8 @@
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="3">
-        <v>44733</v>
+      <c r="B7" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -19692,8 +19701,8 @@
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="3">
-        <v>44733</v>
+      <c r="B8" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
@@ -19725,8 +19734,8 @@
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="3">
-        <v>44733</v>
+      <c r="B9" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
@@ -19758,8 +19767,8 @@
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="3">
-        <v>44733</v>
+      <c r="B10" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
@@ -19791,8 +19800,8 @@
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="3">
-        <v>44733</v>
+      <c r="B11" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
@@ -19824,8 +19833,8 @@
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="3">
-        <v>44733</v>
+      <c r="B12" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
@@ -19857,8 +19866,8 @@
       <c r="A13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="3">
-        <v>44733</v>
+      <c r="B13" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>12</v>
@@ -19890,8 +19899,8 @@
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="3">
-        <v>44733</v>
+      <c r="B14" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>12</v>
@@ -19923,8 +19932,8 @@
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="3">
-        <v>44733</v>
+      <c r="B15" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>12</v>
@@ -19956,8 +19965,8 @@
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="3">
-        <v>44733</v>
+      <c r="B16" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
@@ -19989,8 +19998,8 @@
       <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="3">
-        <v>44733</v>
+      <c r="B17" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>12</v>
@@ -20022,8 +20031,8 @@
       <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="3">
-        <v>44733</v>
+      <c r="B18" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>12</v>
@@ -20057,8 +20066,8 @@
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="3">
-        <v>44733</v>
+      <c r="B19" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
@@ -20092,8 +20101,8 @@
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="3">
-        <v>44733</v>
+      <c r="B20" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>12</v>
@@ -20125,8 +20134,8 @@
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="3">
-        <v>44733</v>
+      <c r="B21" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>12</v>
@@ -20160,8 +20169,8 @@
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="3">
-        <v>44733</v>
+      <c r="B22" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
@@ -20193,8 +20202,8 @@
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="3">
-        <v>44733</v>
+      <c r="B23" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>12</v>
@@ -20226,8 +20235,8 @@
       <c r="A24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="3">
-        <v>44733</v>
+      <c r="B24" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
@@ -20259,8 +20268,8 @@
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="3">
-        <v>44733</v>
+      <c r="B25" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>12</v>
@@ -20292,8 +20301,8 @@
       <c r="A26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="3">
-        <v>44733</v>
+      <c r="B26" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>12</v>
@@ -20325,8 +20334,8 @@
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="3">
-        <v>44733</v>
+      <c r="B27" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
@@ -20358,8 +20367,8 @@
       <c r="A28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="3">
-        <v>44733</v>
+      <c r="B28" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>12</v>
@@ -20391,8 +20400,8 @@
       <c r="A29" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="3">
-        <v>44733</v>
+      <c r="B29" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>12</v>
@@ -20426,8 +20435,8 @@
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="3">
-        <v>44733</v>
+      <c r="B30" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>12</v>
@@ -20459,8 +20468,8 @@
       <c r="A31" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="3">
-        <v>44733</v>
+      <c r="B31" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>12</v>
@@ -20492,8 +20501,8 @@
       <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="3">
-        <v>44733</v>
+      <c r="B32" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>12</v>
@@ -20525,8 +20534,8 @@
       <c r="A33" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="3">
-        <v>44733</v>
+      <c r="B33" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>12</v>
@@ -20558,8 +20567,8 @@
       <c r="A34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="3">
-        <v>44733</v>
+      <c r="B34" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>12</v>
@@ -20591,8 +20600,8 @@
       <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="3">
-        <v>44733</v>
+      <c r="B35" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>12</v>
@@ -20624,8 +20633,8 @@
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="3">
-        <v>44733</v>
+      <c r="B36" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>12</v>
@@ -20657,8 +20666,8 @@
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="3">
-        <v>44733</v>
+      <c r="B37" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>12</v>
@@ -20690,8 +20699,8 @@
       <c r="A38" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="3">
-        <v>44733</v>
+      <c r="B38" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>12</v>
@@ -20725,8 +20734,8 @@
       <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="3">
-        <v>44733</v>
+      <c r="B39" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>12</v>
@@ -20760,8 +20769,8 @@
       <c r="A40" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B40" s="3">
-        <v>44733</v>
+      <c r="B40" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>12</v>
@@ -20793,8 +20802,8 @@
       <c r="A41" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="3">
-        <v>44733</v>
+      <c r="B41" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>12</v>
@@ -20826,8 +20835,8 @@
       <c r="A42" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B42" s="3">
-        <v>44733</v>
+      <c r="B42" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>12</v>
@@ -20859,8 +20868,8 @@
       <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="3">
-        <v>44733</v>
+      <c r="B43" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>12</v>
@@ -20894,8 +20903,8 @@
       <c r="A44" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="3">
-        <v>44733</v>
+      <c r="B44" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>12</v>
@@ -20927,8 +20936,8 @@
       <c r="A45" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="3">
-        <v>44733</v>
+      <c r="B45" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>12</v>
@@ -20962,8 +20971,8 @@
       <c r="A46" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B46" s="3">
-        <v>44733</v>
+      <c r="B46" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>12</v>
@@ -20995,8 +21004,8 @@
       <c r="A47" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="3">
-        <v>44733</v>
+      <c r="B47" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>12</v>
@@ -21028,8 +21037,8 @@
       <c r="A48" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="3">
-        <v>44733</v>
+      <c r="B48" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>12</v>
@@ -21061,8 +21070,8 @@
       <c r="A49" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="3">
-        <v>44733</v>
+      <c r="B49" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>12</v>
@@ -21094,8 +21103,8 @@
       <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B50" s="3">
-        <v>44733</v>
+      <c r="B50" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>12</v>
@@ -21127,8 +21136,8 @@
       <c r="A51" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="3">
-        <v>44733</v>
+      <c r="B51" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>12</v>
@@ -21160,8 +21169,8 @@
       <c r="A52" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="3">
-        <v>44733</v>
+      <c r="B52" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>12</v>
@@ -21193,8 +21202,8 @@
       <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="3">
-        <v>44733</v>
+      <c r="B53" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>12</v>
@@ -21226,8 +21235,8 @@
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="3">
-        <v>44733</v>
+      <c r="B54" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>12</v>
@@ -21259,8 +21268,8 @@
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="3">
-        <v>44733</v>
+      <c r="B55" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>12</v>
@@ -21292,8 +21301,8 @@
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="3">
-        <v>44733</v>
+      <c r="B56" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>12</v>
@@ -21325,8 +21334,8 @@
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="3">
-        <v>44733</v>
+      <c r="B57" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>12</v>
@@ -21358,8 +21367,8 @@
       <c r="A58" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="3">
-        <v>44733</v>
+      <c r="B58" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>12</v>
@@ -21391,8 +21400,8 @@
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="3">
-        <v>44733</v>
+      <c r="B59" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>12</v>
@@ -21424,8 +21433,8 @@
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="3">
-        <v>44733</v>
+      <c r="B60" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>12</v>
@@ -21457,8 +21466,8 @@
       <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="3">
-        <v>44733</v>
+      <c r="B61" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>12</v>
@@ -21490,8 +21499,8 @@
       <c r="A62" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="3">
-        <v>44733</v>
+      <c r="B62" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>31</v>
@@ -21523,8 +21532,8 @@
       <c r="A63" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B63" s="3">
-        <v>44733</v>
+      <c r="B63" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>31</v>
@@ -21556,8 +21565,8 @@
       <c r="A64" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="3">
-        <v>44733</v>
+      <c r="B64" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>31</v>
@@ -21589,8 +21598,8 @@
       <c r="A65" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="3">
-        <v>44733</v>
+      <c r="B65" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>31</v>
@@ -21622,8 +21631,8 @@
       <c r="A66" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B66" s="3">
-        <v>44733</v>
+      <c r="B66" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>31</v>
@@ -21655,8 +21664,8 @@
       <c r="A67" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B67" s="3">
-        <v>44733</v>
+      <c r="B67" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>31</v>
@@ -21688,8 +21697,8 @@
       <c r="A68" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B68" s="3">
-        <v>44733</v>
+      <c r="B68" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>31</v>
@@ -21721,8 +21730,8 @@
       <c r="A69" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B69" s="3">
-        <v>44733</v>
+      <c r="B69" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>31</v>
@@ -21754,8 +21763,8 @@
       <c r="A70" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B70" s="3">
-        <v>44733</v>
+      <c r="B70" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>31</v>
@@ -21787,8 +21796,8 @@
       <c r="A71" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B71" s="3">
-        <v>44733</v>
+      <c r="B71" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>31</v>
@@ -21820,8 +21829,8 @@
       <c r="A72" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B72" s="3">
-        <v>44733</v>
+      <c r="B72" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>31</v>
@@ -21853,8 +21862,8 @@
       <c r="A73" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B73" s="3">
-        <v>44733</v>
+      <c r="B73" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>31</v>
@@ -21886,8 +21895,8 @@
       <c r="A74" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B74" s="3">
-        <v>44733</v>
+      <c r="B74" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>31</v>
@@ -21919,8 +21928,8 @@
       <c r="A75" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B75" s="3">
-        <v>44733</v>
+      <c r="B75" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>31</v>
@@ -21952,8 +21961,8 @@
       <c r="A76" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B76" s="3">
-        <v>44733</v>
+      <c r="B76" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>31</v>
@@ -21985,8 +21994,8 @@
       <c r="A77" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B77" s="3">
-        <v>44733</v>
+      <c r="B77" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>31</v>
@@ -22018,8 +22027,8 @@
       <c r="A78" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B78" s="3">
-        <v>44733</v>
+      <c r="B78" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>31</v>
@@ -22051,8 +22060,8 @@
       <c r="A79" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B79" s="3">
-        <v>44733</v>
+      <c r="B79" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>31</v>
@@ -22084,8 +22093,8 @@
       <c r="A80" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B80" s="3">
-        <v>44733</v>
+      <c r="B80" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>31</v>
@@ -22117,8 +22126,8 @@
       <c r="A81" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B81" s="3">
-        <v>44733</v>
+      <c r="B81" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>31</v>
@@ -22150,8 +22159,8 @@
       <c r="A82" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B82" s="3">
-        <v>44733</v>
+      <c r="B82" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>31</v>
@@ -22183,8 +22192,8 @@
       <c r="A83" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B83" s="3">
-        <v>44733</v>
+      <c r="B83" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>31</v>
@@ -22216,8 +22225,8 @@
       <c r="A84" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B84" s="3">
-        <v>44733</v>
+      <c r="B84" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>31</v>
@@ -22249,8 +22258,8 @@
       <c r="A85" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B85" s="3">
-        <v>44733</v>
+      <c r="B85" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>31</v>
@@ -22282,8 +22291,8 @@
       <c r="A86" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B86" s="3">
-        <v>44733</v>
+      <c r="B86" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>31</v>
@@ -22315,8 +22324,8 @@
       <c r="A87" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B87" s="3">
-        <v>44733</v>
+      <c r="B87" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>31</v>
@@ -22348,8 +22357,8 @@
       <c r="A88" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B88" s="3">
-        <v>44733</v>
+      <c r="B88" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>31</v>
@@ -22381,8 +22390,8 @@
       <c r="A89" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B89" s="3">
-        <v>44733</v>
+      <c r="B89" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>31</v>
@@ -22414,8 +22423,8 @@
       <c r="A90" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B90" s="3">
-        <v>44733</v>
+      <c r="B90" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>31</v>
@@ -22447,8 +22456,8 @@
       <c r="A91" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B91" s="3">
-        <v>44733</v>
+      <c r="B91" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>31</v>
@@ -22480,8 +22489,8 @@
       <c r="A92" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B92" s="3">
-        <v>44733</v>
+      <c r="B92" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>31</v>
@@ -22513,8 +22522,8 @@
       <c r="A93" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B93" s="3">
-        <v>44733</v>
+      <c r="B93" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>31</v>
@@ -22546,8 +22555,8 @@
       <c r="A94" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B94" s="3">
-        <v>44733</v>
+      <c r="B94" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>31</v>
@@ -22579,8 +22588,8 @@
       <c r="A95" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B95" s="3">
-        <v>44733</v>
+      <c r="B95" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>31</v>
@@ -22612,8 +22621,8 @@
       <c r="A96" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B96" s="3">
-        <v>44733</v>
+      <c r="B96" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>31</v>
@@ -22645,8 +22654,8 @@
       <c r="A97" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B97" s="3">
-        <v>44733</v>
+      <c r="B97" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>31</v>
@@ -22678,8 +22687,8 @@
       <c r="A98" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B98" s="3">
-        <v>44733</v>
+      <c r="B98" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>31</v>
@@ -22711,8 +22720,8 @@
       <c r="A99" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B99" s="3">
-        <v>44733</v>
+      <c r="B99" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>31</v>
@@ -22744,8 +22753,8 @@
       <c r="A100" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B100" s="3">
-        <v>44733</v>
+      <c r="B100" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>31</v>
@@ -22777,8 +22786,8 @@
       <c r="A101" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B101" s="3">
-        <v>44733</v>
+      <c r="B101" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>31</v>
@@ -22810,8 +22819,8 @@
       <c r="A102" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B102" s="3">
-        <v>44733</v>
+      <c r="B102" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>31</v>
@@ -22843,8 +22852,8 @@
       <c r="A103" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B103" s="3">
-        <v>44733</v>
+      <c r="B103" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>31</v>
@@ -22876,8 +22885,8 @@
       <c r="A104" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B104" s="3">
-        <v>44733</v>
+      <c r="B104" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>31</v>
@@ -22909,8 +22918,8 @@
       <c r="A105" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B105" s="3">
-        <v>44733</v>
+      <c r="B105" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>31</v>
@@ -22942,8 +22951,8 @@
       <c r="A106" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B106" s="3">
-        <v>44733</v>
+      <c r="B106" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>31</v>
@@ -22975,8 +22984,8 @@
       <c r="A107" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B107" s="3">
-        <v>44733</v>
+      <c r="B107" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>31</v>
@@ -23008,8 +23017,8 @@
       <c r="A108" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B108" s="3">
-        <v>44733</v>
+      <c r="B108" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>31</v>
@@ -23041,8 +23050,8 @@
       <c r="A109" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B109" s="3">
-        <v>44733</v>
+      <c r="B109" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>31</v>
@@ -23074,8 +23083,8 @@
       <c r="A110" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B110" s="3">
-        <v>44733</v>
+      <c r="B110" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>31</v>
@@ -23107,8 +23116,8 @@
       <c r="A111" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B111" s="3">
-        <v>44733</v>
+      <c r="B111" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>31</v>
@@ -23140,8 +23149,8 @@
       <c r="A112" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B112" s="3">
-        <v>44733</v>
+      <c r="B112" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>31</v>
@@ -23173,8 +23182,8 @@
       <c r="A113" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B113" s="3">
-        <v>44733</v>
+      <c r="B113" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>31</v>
@@ -23206,8 +23215,8 @@
       <c r="A114" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B114" s="3">
-        <v>44733</v>
+      <c r="B114" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>31</v>
@@ -23239,8 +23248,8 @@
       <c r="A115" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B115" s="3">
-        <v>44733</v>
+      <c r="B115" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>31</v>
@@ -23272,8 +23281,8 @@
       <c r="A116" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B116" s="3">
-        <v>44733</v>
+      <c r="B116" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>31</v>
@@ -23305,8 +23314,8 @@
       <c r="A117" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B117" s="3">
-        <v>44733</v>
+      <c r="B117" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>31</v>
@@ -23338,8 +23347,8 @@
       <c r="A118" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B118" s="3">
-        <v>44733</v>
+      <c r="B118" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>31</v>
@@ -23371,8 +23380,8 @@
       <c r="A119" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B119" s="3">
-        <v>44733</v>
+      <c r="B119" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>31</v>
@@ -23404,8 +23413,8 @@
       <c r="A120" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B120" s="3">
-        <v>44733</v>
+      <c r="B120" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>31</v>
@@ -23437,8 +23446,8 @@
       <c r="A121" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B121" s="3">
-        <v>44733</v>
+      <c r="B121" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>31</v>
@@ -23470,8 +23479,8 @@
       <c r="A122" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B122" s="3">
-        <v>44733</v>
+      <c r="B122" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>12</v>
@@ -23503,8 +23512,8 @@
       <c r="A123" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B123" s="3">
-        <v>44733</v>
+      <c r="B123" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>12</v>
@@ -23536,8 +23545,8 @@
       <c r="A124" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B124" s="3">
-        <v>44733</v>
+      <c r="B124" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>12</v>
@@ -23569,8 +23578,8 @@
       <c r="A125" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B125" s="3">
-        <v>44733</v>
+      <c r="B125" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>12</v>
@@ -23602,8 +23611,8 @@
       <c r="A126" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B126" s="3">
-        <v>44733</v>
+      <c r="B126" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>12</v>
@@ -23635,8 +23644,8 @@
       <c r="A127" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B127" s="3">
-        <v>44733</v>
+      <c r="B127" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>12</v>
@@ -23668,8 +23677,8 @@
       <c r="A128" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B128" s="3">
-        <v>44733</v>
+      <c r="B128" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>12</v>
@@ -23701,8 +23710,8 @@
       <c r="A129" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B129" s="3">
-        <v>44733</v>
+      <c r="B129" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>12</v>
@@ -23734,8 +23743,8 @@
       <c r="A130" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B130" s="3">
-        <v>44733</v>
+      <c r="B130" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>12</v>
@@ -23767,8 +23776,8 @@
       <c r="A131" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B131" s="3">
-        <v>44733</v>
+      <c r="B131" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>12</v>
@@ -23800,8 +23809,8 @@
       <c r="A132" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B132" s="3">
-        <v>44733</v>
+      <c r="B132" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>12</v>
@@ -23833,8 +23842,8 @@
       <c r="A133" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B133" s="3">
-        <v>44733</v>
+      <c r="B133" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>12</v>
@@ -23866,8 +23875,8 @@
       <c r="A134" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B134" s="3">
-        <v>44733</v>
+      <c r="B134" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>12</v>
@@ -23899,8 +23908,8 @@
       <c r="A135" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B135" s="3">
-        <v>44733</v>
+      <c r="B135" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>12</v>
@@ -23932,8 +23941,8 @@
       <c r="A136" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B136" s="3">
-        <v>44733</v>
+      <c r="B136" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>12</v>
@@ -23965,8 +23974,8 @@
       <c r="A137" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B137" s="3">
-        <v>44733</v>
+      <c r="B137" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>12</v>
@@ -23998,8 +24007,8 @@
       <c r="A138" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B138" s="3">
-        <v>44733</v>
+      <c r="B138" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>12</v>
@@ -24031,8 +24040,8 @@
       <c r="A139" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B139" s="3">
-        <v>44733</v>
+      <c r="B139" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>12</v>
@@ -24064,8 +24073,8 @@
       <c r="A140" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B140" s="3">
-        <v>44733</v>
+      <c r="B140" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>12</v>
@@ -24097,8 +24106,8 @@
       <c r="A141" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B141" s="3">
-        <v>44733</v>
+      <c r="B141" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>12</v>
@@ -24136,7 +24145,7 @@
   <dimension ref="A1:K141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G142" sqref="G142"/>
+      <selection activeCell="B2" sqref="B2:B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24191,8 +24200,8 @@
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3">
-        <v>44743</v>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -24224,8 +24233,8 @@
       <c r="A3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="3">
-        <v>44743</v>
+      <c r="B3" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -24257,8 +24266,8 @@
       <c r="A4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="3">
-        <v>44743</v>
+      <c r="B4" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
@@ -24290,8 +24299,8 @@
       <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="3">
-        <v>44743</v>
+      <c r="B5" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
@@ -24323,8 +24332,8 @@
       <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="3">
-        <v>44743</v>
+      <c r="B6" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
@@ -24356,8 +24365,8 @@
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="3">
-        <v>44743</v>
+      <c r="B7" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -24389,8 +24398,8 @@
       <c r="A8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="3">
-        <v>44743</v>
+      <c r="B8" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
@@ -24422,8 +24431,8 @@
       <c r="A9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="3">
-        <v>44743</v>
+      <c r="B9" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
@@ -24455,8 +24464,8 @@
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="3">
-        <v>44743</v>
+      <c r="B10" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
@@ -24488,8 +24497,8 @@
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="3">
-        <v>44743</v>
+      <c r="B11" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
@@ -24521,8 +24530,8 @@
       <c r="A12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="3">
-        <v>44743</v>
+      <c r="B12" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
@@ -24554,8 +24563,8 @@
       <c r="A13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="3">
-        <v>44743</v>
+      <c r="B13" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>12</v>
@@ -24587,8 +24596,8 @@
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="3">
-        <v>44743</v>
+      <c r="B14" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>12</v>
@@ -24620,8 +24629,8 @@
       <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="3">
-        <v>44743</v>
+      <c r="B15" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>12</v>
@@ -24653,8 +24662,8 @@
       <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="3">
-        <v>44743</v>
+      <c r="B16" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
@@ -24686,8 +24695,8 @@
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="3">
-        <v>44743</v>
+      <c r="B17" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>12</v>
@@ -24719,8 +24728,8 @@
       <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="3">
-        <v>44743</v>
+      <c r="B18" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>12</v>
@@ -24754,8 +24763,8 @@
       <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="3">
-        <v>44743</v>
+      <c r="B19" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
@@ -24789,8 +24798,8 @@
       <c r="A20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="3">
-        <v>44743</v>
+      <c r="B20" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>12</v>
@@ -24824,8 +24833,8 @@
       <c r="A21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="3">
-        <v>44743</v>
+      <c r="B21" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>12</v>
@@ -24859,8 +24868,8 @@
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="3">
-        <v>44743</v>
+      <c r="B22" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
@@ -24892,8 +24901,8 @@
       <c r="A23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="3">
-        <v>44743</v>
+      <c r="B23" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>12</v>
@@ -24925,8 +24934,8 @@
       <c r="A24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="3">
-        <v>44743</v>
+      <c r="B24" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
@@ -24958,8 +24967,8 @@
       <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="3">
-        <v>44743</v>
+      <c r="B25" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>12</v>
@@ -24991,8 +25000,8 @@
       <c r="A26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="3">
-        <v>44743</v>
+      <c r="B26" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>12</v>
@@ -25024,8 +25033,8 @@
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="3">
-        <v>44743</v>
+      <c r="B27" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
@@ -25057,8 +25066,8 @@
       <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="3">
-        <v>44743</v>
+      <c r="B28" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>12</v>
@@ -25090,8 +25099,8 @@
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="3">
-        <v>44743</v>
+      <c r="B29" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>12</v>
@@ -25123,8 +25132,8 @@
       <c r="A30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="3">
-        <v>44743</v>
+      <c r="B30" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>12</v>
@@ -25156,8 +25165,8 @@
       <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="3">
-        <v>44743</v>
+      <c r="B31" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>12</v>
@@ -25189,8 +25198,8 @@
       <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="3">
-        <v>44743</v>
+      <c r="B32" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>12</v>
@@ -25222,8 +25231,8 @@
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="3">
-        <v>44743</v>
+      <c r="B33" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>12</v>
@@ -25255,8 +25264,8 @@
       <c r="A34" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B34" s="3">
-        <v>44743</v>
+      <c r="B34" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>12</v>
@@ -25288,8 +25297,8 @@
       <c r="A35" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="3">
-        <v>44743</v>
+      <c r="B35" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>12</v>
@@ -25321,8 +25330,8 @@
       <c r="A36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="3">
-        <v>44743</v>
+      <c r="B36" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>12</v>
@@ -25354,8 +25363,8 @@
       <c r="A37" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B37" s="3">
-        <v>44743</v>
+      <c r="B37" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>12</v>
@@ -25387,8 +25396,8 @@
       <c r="A38" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B38" s="3">
-        <v>44743</v>
+      <c r="B38" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>12</v>
@@ -25422,8 +25431,8 @@
       <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="3">
-        <v>44743</v>
+      <c r="B39" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>12</v>
@@ -25457,8 +25466,8 @@
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="3">
-        <v>44743</v>
+      <c r="B40" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>12</v>
@@ -25492,8 +25501,8 @@
       <c r="A41" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="3">
-        <v>44743</v>
+      <c r="B41" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>12</v>
@@ -25527,8 +25536,8 @@
       <c r="A42" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="3">
-        <v>44743</v>
+      <c r="B42" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>12</v>
@@ -25562,8 +25571,8 @@
       <c r="A43" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="3">
-        <v>44743</v>
+      <c r="B43" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>12</v>
@@ -25597,8 +25606,8 @@
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="3">
-        <v>44743</v>
+      <c r="B44" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>12</v>
@@ -25632,8 +25641,8 @@
       <c r="A45" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B45" s="3">
-        <v>44743</v>
+      <c r="B45" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>12</v>
@@ -25667,8 +25676,8 @@
       <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="3">
-        <v>44743</v>
+      <c r="B46" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>12</v>
@@ -25700,8 +25709,8 @@
       <c r="A47" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B47" s="3">
-        <v>44743</v>
+      <c r="B47" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>12</v>
@@ -25733,8 +25742,8 @@
       <c r="A48" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="3">
-        <v>44743</v>
+      <c r="B48" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>12</v>
@@ -25766,8 +25775,8 @@
       <c r="A49" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B49" s="3">
-        <v>44743</v>
+      <c r="B49" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>12</v>
@@ -25799,8 +25808,8 @@
       <c r="A50" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B50" s="3">
-        <v>44743</v>
+      <c r="B50" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>12</v>
@@ -25832,8 +25841,8 @@
       <c r="A51" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B51" s="3">
-        <v>44743</v>
+      <c r="B51" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>12</v>
@@ -25865,8 +25874,8 @@
       <c r="A52" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="3">
-        <v>44743</v>
+      <c r="B52" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>12</v>
@@ -25898,8 +25907,8 @@
       <c r="A53" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="3">
-        <v>44743</v>
+      <c r="B53" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>12</v>
@@ -25931,8 +25940,8 @@
       <c r="A54" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="3">
-        <v>44743</v>
+      <c r="B54" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>12</v>
@@ -25964,8 +25973,8 @@
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B55" s="3">
-        <v>44743</v>
+      <c r="B55" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>12</v>
@@ -25997,8 +26006,8 @@
       <c r="A56" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B56" s="3">
-        <v>44743</v>
+      <c r="B56" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>12</v>
@@ -26030,8 +26039,8 @@
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="3">
-        <v>44743</v>
+      <c r="B57" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>12</v>
@@ -26063,8 +26072,8 @@
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="3">
-        <v>44743</v>
+      <c r="B58" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>12</v>
@@ -26098,8 +26107,8 @@
       <c r="A59" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="3">
-        <v>44743</v>
+      <c r="B59" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>12</v>
@@ -26131,8 +26140,8 @@
       <c r="A60" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="3">
-        <v>44743</v>
+      <c r="B60" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>12</v>
@@ -26166,8 +26175,8 @@
       <c r="A61" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="3">
-        <v>44743</v>
+      <c r="B61" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>12</v>
@@ -26199,8 +26208,8 @@
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="3">
-        <v>44743</v>
+      <c r="B62" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>31</v>
@@ -26232,8 +26241,8 @@
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B63" s="3">
-        <v>44743</v>
+      <c r="B63" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>31</v>
@@ -26265,8 +26274,8 @@
       <c r="A64" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="3">
-        <v>44743</v>
+      <c r="B64" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>31</v>
@@ -26298,8 +26307,8 @@
       <c r="A65" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="3">
-        <v>44743</v>
+      <c r="B65" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>31</v>
@@ -26331,8 +26340,8 @@
       <c r="A66" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B66" s="3">
-        <v>44743</v>
+      <c r="B66" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>31</v>
@@ -26364,8 +26373,8 @@
       <c r="A67" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B67" s="3">
-        <v>44743</v>
+      <c r="B67" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>31</v>
@@ -26397,8 +26406,8 @@
       <c r="A68" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="3">
-        <v>44743</v>
+      <c r="B68" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>31</v>
@@ -26430,8 +26439,8 @@
       <c r="A69" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B69" s="3">
-        <v>44743</v>
+      <c r="B69" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>31</v>
@@ -26463,8 +26472,8 @@
       <c r="A70" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="3">
-        <v>44743</v>
+      <c r="B70" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>31</v>
@@ -26496,8 +26505,8 @@
       <c r="A71" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B71" s="3">
-        <v>44743</v>
+      <c r="B71" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>31</v>
@@ -26531,8 +26540,8 @@
       <c r="A72" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B72" s="3">
-        <v>44743</v>
+      <c r="B72" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>31</v>
@@ -26564,8 +26573,8 @@
       <c r="A73" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B73" s="3">
-        <v>44743</v>
+      <c r="B73" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>31</v>
@@ -26599,8 +26608,8 @@
       <c r="A74" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="3">
-        <v>44743</v>
+      <c r="B74" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>31</v>
@@ -26632,8 +26641,8 @@
       <c r="A75" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B75" s="3">
-        <v>44743</v>
+      <c r="B75" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>31</v>
@@ -26665,8 +26674,8 @@
       <c r="A76" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B76" s="3">
-        <v>44743</v>
+      <c r="B76" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>31</v>
@@ -26698,8 +26707,8 @@
       <c r="A77" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B77" s="3">
-        <v>44743</v>
+      <c r="B77" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>31</v>
@@ -26731,8 +26740,8 @@
       <c r="A78" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B78" s="3">
-        <v>44743</v>
+      <c r="B78" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>31</v>
@@ -26764,8 +26773,8 @@
       <c r="A79" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B79" s="3">
-        <v>44743</v>
+      <c r="B79" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>31</v>
@@ -26797,8 +26806,8 @@
       <c r="A80" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B80" s="3">
-        <v>44743</v>
+      <c r="B80" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>31</v>
@@ -26830,8 +26839,8 @@
       <c r="A81" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B81" s="3">
-        <v>44743</v>
+      <c r="B81" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>31</v>
@@ -26863,8 +26872,8 @@
       <c r="A82" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B82" s="3">
-        <v>44743</v>
+      <c r="B82" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>31</v>
@@ -26896,8 +26905,8 @@
       <c r="A83" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B83" s="3">
-        <v>44743</v>
+      <c r="B83" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>31</v>
@@ -26929,8 +26938,8 @@
       <c r="A84" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B84" s="3">
-        <v>44743</v>
+      <c r="B84" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>31</v>
@@ -26962,8 +26971,8 @@
       <c r="A85" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B85" s="3">
-        <v>44743</v>
+      <c r="B85" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>31</v>
@@ -26995,8 +27004,8 @@
       <c r="A86" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B86" s="3">
-        <v>44743</v>
+      <c r="B86" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>31</v>
@@ -27028,8 +27037,8 @@
       <c r="A87" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B87" s="3">
-        <v>44743</v>
+      <c r="B87" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>31</v>
@@ -27061,8 +27070,8 @@
       <c r="A88" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B88" s="3">
-        <v>44743</v>
+      <c r="B88" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>31</v>
@@ -27094,8 +27103,8 @@
       <c r="A89" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B89" s="3">
-        <v>44743</v>
+      <c r="B89" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>31</v>
@@ -27127,8 +27136,8 @@
       <c r="A90" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B90" s="3">
-        <v>44743</v>
+      <c r="B90" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>31</v>
@@ -27160,8 +27169,8 @@
       <c r="A91" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B91" s="3">
-        <v>44743</v>
+      <c r="B91" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>31</v>
@@ -27193,8 +27202,8 @@
       <c r="A92" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B92" s="3">
-        <v>44743</v>
+      <c r="B92" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>31</v>
@@ -27226,8 +27235,8 @@
       <c r="A93" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B93" s="3">
-        <v>44743</v>
+      <c r="B93" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>31</v>
@@ -27259,8 +27268,8 @@
       <c r="A94" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B94" s="3">
-        <v>44743</v>
+      <c r="B94" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>31</v>
@@ -27292,8 +27301,8 @@
       <c r="A95" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B95" s="3">
-        <v>44743</v>
+      <c r="B95" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>31</v>
@@ -27325,8 +27334,8 @@
       <c r="A96" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B96" s="3">
-        <v>44743</v>
+      <c r="B96" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>31</v>
@@ -27358,8 +27367,8 @@
       <c r="A97" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B97" s="3">
-        <v>44743</v>
+      <c r="B97" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>31</v>
@@ -27391,8 +27400,8 @@
       <c r="A98" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B98" s="3">
-        <v>44743</v>
+      <c r="B98" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>31</v>
@@ -27424,8 +27433,8 @@
       <c r="A99" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B99" s="3">
-        <v>44743</v>
+      <c r="B99" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>31</v>
@@ -27457,8 +27466,8 @@
       <c r="A100" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B100" s="3">
-        <v>44743</v>
+      <c r="B100" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>31</v>
@@ -27490,8 +27499,8 @@
       <c r="A101" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B101" s="3">
-        <v>44743</v>
+      <c r="B101" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>31</v>
@@ -27523,8 +27532,8 @@
       <c r="A102" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B102" s="3">
-        <v>44743</v>
+      <c r="B102" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>31</v>
@@ -27556,8 +27565,8 @@
       <c r="A103" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B103" s="3">
-        <v>44743</v>
+      <c r="B103" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>31</v>
@@ -27589,8 +27598,8 @@
       <c r="A104" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B104" s="3">
-        <v>44743</v>
+      <c r="B104" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>31</v>
@@ -27622,8 +27631,8 @@
       <c r="A105" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B105" s="3">
-        <v>44743</v>
+      <c r="B105" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>31</v>
@@ -27655,8 +27664,8 @@
       <c r="A106" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B106" s="3">
-        <v>44743</v>
+      <c r="B106" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>31</v>
@@ -27688,8 +27697,8 @@
       <c r="A107" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B107" s="3">
-        <v>44743</v>
+      <c r="B107" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>31</v>
@@ -27721,8 +27730,8 @@
       <c r="A108" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B108" s="3">
-        <v>44743</v>
+      <c r="B108" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>31</v>
@@ -27754,8 +27763,8 @@
       <c r="A109" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B109" s="3">
-        <v>44743</v>
+      <c r="B109" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>31</v>
@@ -27787,8 +27796,8 @@
       <c r="A110" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B110" s="3">
-        <v>44743</v>
+      <c r="B110" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>31</v>
@@ -27820,8 +27829,8 @@
       <c r="A111" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B111" s="3">
-        <v>44743</v>
+      <c r="B111" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>31</v>
@@ -27853,8 +27862,8 @@
       <c r="A112" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B112" s="3">
-        <v>44743</v>
+      <c r="B112" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>31</v>
@@ -27886,8 +27895,8 @@
       <c r="A113" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B113" s="3">
-        <v>44743</v>
+      <c r="B113" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>31</v>
@@ -27919,8 +27928,8 @@
       <c r="A114" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B114" s="3">
-        <v>44743</v>
+      <c r="B114" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>31</v>
@@ -27952,8 +27961,8 @@
       <c r="A115" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B115" s="3">
-        <v>44743</v>
+      <c r="B115" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>31</v>
@@ -27985,8 +27994,8 @@
       <c r="A116" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B116" s="3">
-        <v>44743</v>
+      <c r="B116" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>31</v>
@@ -28018,8 +28027,8 @@
       <c r="A117" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B117" s="3">
-        <v>44743</v>
+      <c r="B117" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>31</v>
@@ -28051,8 +28060,8 @@
       <c r="A118" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B118" s="3">
-        <v>44743</v>
+      <c r="B118" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>31</v>
@@ -28084,8 +28093,8 @@
       <c r="A119" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B119" s="3">
-        <v>44743</v>
+      <c r="B119" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>31</v>
@@ -28117,8 +28126,8 @@
       <c r="A120" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B120" s="3">
-        <v>44743</v>
+      <c r="B120" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>31</v>
@@ -28150,8 +28159,8 @@
       <c r="A121" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B121" s="3">
-        <v>44743</v>
+      <c r="B121" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>31</v>
@@ -28183,8 +28192,8 @@
       <c r="A122" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B122" s="3">
-        <v>44743</v>
+      <c r="B122" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>12</v>
@@ -28216,8 +28225,8 @@
       <c r="A123" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B123" s="3">
-        <v>44743</v>
+      <c r="B123" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>12</v>
@@ -28249,8 +28258,8 @@
       <c r="A124" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B124" s="3">
-        <v>44743</v>
+      <c r="B124" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>12</v>
@@ -28282,8 +28291,8 @@
       <c r="A125" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B125" s="3">
-        <v>44743</v>
+      <c r="B125" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>12</v>
@@ -28315,8 +28324,8 @@
       <c r="A126" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B126" s="3">
-        <v>44743</v>
+      <c r="B126" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>12</v>
@@ -28348,8 +28357,8 @@
       <c r="A127" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B127" s="3">
-        <v>44743</v>
+      <c r="B127" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>12</v>
@@ -28381,8 +28390,8 @@
       <c r="A128" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B128" s="3">
-        <v>44743</v>
+      <c r="B128" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>12</v>
@@ -28414,8 +28423,8 @@
       <c r="A129" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B129" s="3">
-        <v>44743</v>
+      <c r="B129" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>12</v>
@@ -28447,8 +28456,8 @@
       <c r="A130" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B130" s="3">
-        <v>44743</v>
+      <c r="B130" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>12</v>
@@ -28480,8 +28489,8 @@
       <c r="A131" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B131" s="3">
-        <v>44743</v>
+      <c r="B131" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>12</v>
@@ -28513,8 +28522,8 @@
       <c r="A132" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B132" s="3">
-        <v>44743</v>
+      <c r="B132" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>12</v>
@@ -28546,8 +28555,8 @@
       <c r="A133" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B133" s="3">
-        <v>44743</v>
+      <c r="B133" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>12</v>
@@ -28579,8 +28588,8 @@
       <c r="A134" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B134" s="3">
-        <v>44743</v>
+      <c r="B134" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>12</v>
@@ -28612,8 +28621,8 @@
       <c r="A135" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B135" s="3">
-        <v>44743</v>
+      <c r="B135" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>12</v>
@@ -28645,8 +28654,8 @@
       <c r="A136" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B136" s="3">
-        <v>44743</v>
+      <c r="B136" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>12</v>
@@ -28678,8 +28687,8 @@
       <c r="A137" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B137" s="3">
-        <v>44743</v>
+      <c r="B137" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>12</v>
@@ -28711,8 +28720,8 @@
       <c r="A138" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B138" s="3">
-        <v>44743</v>
+      <c r="B138" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>12</v>
@@ -28744,8 +28753,8 @@
       <c r="A139" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B139" s="3">
-        <v>44743</v>
+      <c r="B139" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>12</v>
@@ -28777,8 +28786,8 @@
       <c r="A140" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B140" s="3">
-        <v>44743</v>
+      <c r="B140" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>12</v>
@@ -28810,8 +28819,8 @@
       <c r="A141" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B141" s="3">
-        <v>44743</v>
+      <c r="B141" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>12</v>
@@ -28848,8 +28857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57C79E-F215-4103-AD42-D55276101BC9}">
   <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28900,8 +28909,8 @@
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="3">
-        <v>44749</v>
+      <c r="B2" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>12</v>
@@ -28933,8 +28942,8 @@
       <c r="A3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="3">
-        <v>44749</v>
+      <c r="B3" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -28966,8 +28975,8 @@
       <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="3">
-        <v>44749</v>
+      <c r="B4" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
@@ -28999,8 +29008,8 @@
       <c r="A5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="3">
-        <v>44749</v>
+      <c r="B5" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
@@ -29032,8 +29041,8 @@
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="3">
-        <v>44749</v>
+      <c r="B6" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
@@ -29065,8 +29074,8 @@
       <c r="A7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="3">
-        <v>44749</v>
+      <c r="B7" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -29098,8 +29107,8 @@
       <c r="A8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="3">
-        <v>44749</v>
+      <c r="B8" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
@@ -29131,8 +29140,8 @@
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="3">
-        <v>44749</v>
+      <c r="B9" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
@@ -29164,8 +29173,8 @@
       <c r="A10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="3">
-        <v>44749</v>
+      <c r="B10" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
@@ -29197,8 +29206,8 @@
       <c r="A11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="3">
-        <v>44749</v>
+      <c r="B11" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
@@ -29230,8 +29239,8 @@
       <c r="A12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="3">
-        <v>44749</v>
+      <c r="B12" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
@@ -29263,8 +29272,8 @@
       <c r="A13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="3">
-        <v>44749</v>
+      <c r="B13" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>12</v>
@@ -29296,8 +29305,8 @@
       <c r="A14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="3">
-        <v>44749</v>
+      <c r="B14" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>12</v>
@@ -29329,8 +29338,8 @@
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="3">
-        <v>44749</v>
+      <c r="B15" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>12</v>
@@ -29362,8 +29371,8 @@
       <c r="A16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="3">
-        <v>44749</v>
+      <c r="B16" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
@@ -29395,8 +29404,8 @@
       <c r="A17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="3">
-        <v>44749</v>
+      <c r="B17" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>12</v>
@@ -29428,8 +29437,8 @@
       <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="3">
-        <v>44749</v>
+      <c r="B18" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>12</v>
@@ -29463,8 +29472,8 @@
       <c r="A19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="3">
-        <v>44749</v>
+      <c r="B19" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>12</v>
@@ -29498,8 +29507,8 @@
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="3">
-        <v>44749</v>
+      <c r="B20" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>12</v>
@@ -29533,8 +29542,8 @@
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="3">
-        <v>44749</v>
+      <c r="B21" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>12</v>
@@ -29568,8 +29577,8 @@
       <c r="A22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="3">
-        <v>44749</v>
+      <c r="B22" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
@@ -29601,8 +29610,8 @@
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="3">
-        <v>44749</v>
+      <c r="B23" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>12</v>
@@ -29634,8 +29643,8 @@
       <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="3">
-        <v>44749</v>
+      <c r="B24" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
@@ -29667,8 +29676,8 @@
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="3">
-        <v>44749</v>
+      <c r="B25" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>12</v>
@@ -29700,8 +29709,8 @@
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="3">
-        <v>44749</v>
+      <c r="B26" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>12</v>
@@ -29735,8 +29744,8 @@
       <c r="A27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="3">
-        <v>44749</v>
+      <c r="B27" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>12</v>
@@ -29768,8 +29777,8 @@
       <c r="A28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="3">
-        <v>44749</v>
+      <c r="B28" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>12</v>
@@ -29801,8 +29810,8 @@
       <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="3">
-        <v>44749</v>
+      <c r="B29" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>12</v>
@@ -29836,8 +29845,8 @@
       <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="3">
-        <v>44749</v>
+      <c r="B30" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>12</v>
@@ -29869,8 +29878,8 @@
       <c r="A31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="3">
-        <v>44749</v>
+      <c r="B31" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>12</v>
@@ -29902,8 +29911,8 @@
       <c r="A32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="3">
-        <v>44749</v>
+      <c r="B32" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>12</v>
@@ -29935,8 +29944,8 @@
       <c r="A33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="3">
-        <v>44749</v>
+      <c r="B33" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>12</v>
@@ -29968,8 +29977,8 @@
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="3">
-        <v>44749</v>
+      <c r="B34" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>12</v>
@@ -30001,8 +30010,8 @@
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="3">
-        <v>44749</v>
+      <c r="B35" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>12</v>
@@ -30034,8 +30043,8 @@
       <c r="A36" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B36" s="3">
-        <v>44749</v>
+      <c r="B36" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>12</v>
@@ -30067,8 +30076,8 @@
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="3">
-        <v>44749</v>
+      <c r="B37" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>12</v>
@@ -30100,8 +30109,8 @@
       <c r="A38" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="3">
-        <v>44749</v>
+      <c r="B38" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>12</v>
@@ -30135,8 +30144,8 @@
       <c r="A39" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="3">
-        <v>44749</v>
+      <c r="B39" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>12</v>
@@ -30170,8 +30179,8 @@
       <c r="A40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="3">
-        <v>44749</v>
+      <c r="B40" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>12</v>
@@ -30205,8 +30214,8 @@
       <c r="A41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="3">
-        <v>44749</v>
+      <c r="B41" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>12</v>
@@ -30238,8 +30247,8 @@
       <c r="A42" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B42" s="3">
-        <v>44749</v>
+      <c r="B42" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>12</v>
@@ -30271,8 +30280,8 @@
       <c r="A43" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="3">
-        <v>44749</v>
+      <c r="B43" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>12</v>
@@ -30306,8 +30315,8 @@
       <c r="A44" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="3">
-        <v>44749</v>
+      <c r="B44" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>12</v>
@@ -30339,8 +30348,8 @@
       <c r="A45" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="3">
-        <v>44749</v>
+      <c r="B45" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>12</v>
@@ -30374,8 +30383,8 @@
       <c r="A46" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="3">
-        <v>44749</v>
+      <c r="B46" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>12</v>
@@ -30407,8 +30416,8 @@
       <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="3">
-        <v>44749</v>
+      <c r="B47" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>12</v>
@@ -30440,8 +30449,8 @@
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="3">
-        <v>44749</v>
+      <c r="B48" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>12</v>
@@ -30473,8 +30482,8 @@
       <c r="A49" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B49" s="3">
-        <v>44749</v>
+      <c r="B49" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>12</v>
@@ -30506,8 +30515,8 @@
       <c r="A50" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="3">
-        <v>44749</v>
+      <c r="B50" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>12</v>
@@ -30539,8 +30548,8 @@
       <c r="A51" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B51" s="3">
-        <v>44749</v>
+      <c r="B51" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>12</v>
@@ -30572,8 +30581,8 @@
       <c r="A52" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B52" s="3">
-        <v>44749</v>
+      <c r="B52" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>12</v>
@@ -30605,8 +30614,8 @@
       <c r="A53" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B53" s="3">
-        <v>44749</v>
+      <c r="B53" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>12</v>
@@ -30638,8 +30647,8 @@
       <c r="A54" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="3">
-        <v>44749</v>
+      <c r="B54" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>12</v>
@@ -30671,8 +30680,8 @@
       <c r="A55" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B55" s="3">
-        <v>44749</v>
+      <c r="B55" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>12</v>
@@ -30704,8 +30713,8 @@
       <c r="A56" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="3">
-        <v>44749</v>
+      <c r="B56" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>12</v>
@@ -30737,8 +30746,8 @@
       <c r="A57" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="3">
-        <v>44749</v>
+      <c r="B57" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>12</v>
@@ -30770,8 +30779,8 @@
       <c r="A58" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B58" s="3">
-        <v>44749</v>
+      <c r="B58" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>12</v>
@@ -30803,8 +30812,8 @@
       <c r="A59" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="3">
-        <v>44749</v>
+      <c r="B59" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>12</v>
@@ -30836,8 +30845,8 @@
       <c r="A60" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="3">
-        <v>44749</v>
+      <c r="B60" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>12</v>
@@ -30869,8 +30878,8 @@
       <c r="A61" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B61" s="3">
-        <v>44749</v>
+      <c r="B61" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>12</v>
@@ -30902,8 +30911,8 @@
       <c r="A62" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="3">
-        <v>44749</v>
+      <c r="B62" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>31</v>
@@ -30935,8 +30944,8 @@
       <c r="A63" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="3">
-        <v>44749</v>
+      <c r="B63" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>31</v>
@@ -30968,8 +30977,8 @@
       <c r="A64" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="3">
-        <v>44749</v>
+      <c r="B64" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>31</v>
@@ -31001,8 +31010,8 @@
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="3">
-        <v>44749</v>
+      <c r="B65" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>31</v>
@@ -31034,8 +31043,8 @@
       <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="3">
-        <v>44749</v>
+      <c r="B66" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>31</v>
@@ -31067,8 +31076,8 @@
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="3">
-        <v>44749</v>
+      <c r="B67" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>31</v>
@@ -31100,8 +31109,8 @@
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="3">
-        <v>44749</v>
+      <c r="B68" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>31</v>
@@ -31133,8 +31142,8 @@
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B69" s="3">
-        <v>44749</v>
+      <c r="B69" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>31</v>
@@ -31166,8 +31175,8 @@
       <c r="A70" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B70" s="3">
-        <v>44749</v>
+      <c r="B70" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>31</v>
@@ -31199,8 +31208,8 @@
       <c r="A71" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B71" s="3">
-        <v>44749</v>
+      <c r="B71" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>31</v>
@@ -31232,8 +31241,8 @@
       <c r="A72" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B72" s="3">
-        <v>44749</v>
+      <c r="B72" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>31</v>
@@ -31265,8 +31274,8 @@
       <c r="A73" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B73" s="3">
-        <v>44749</v>
+      <c r="B73" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>31</v>
@@ -31298,8 +31307,8 @@
       <c r="A74" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B74" s="3">
-        <v>44749</v>
+      <c r="B74" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>31</v>
@@ -31331,8 +31340,8 @@
       <c r="A75" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B75" s="3">
-        <v>44749</v>
+      <c r="B75" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>31</v>
@@ -31364,8 +31373,8 @@
       <c r="A76" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B76" s="3">
-        <v>44749</v>
+      <c r="B76" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>31</v>
@@ -31397,8 +31406,8 @@
       <c r="A77" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B77" s="3">
-        <v>44749</v>
+      <c r="B77" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>31</v>
@@ -31430,8 +31439,8 @@
       <c r="A78" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B78" s="3">
-        <v>44749</v>
+      <c r="B78" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>31</v>
@@ -31463,8 +31472,8 @@
       <c r="A79" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B79" s="3">
-        <v>44749</v>
+      <c r="B79" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>31</v>
@@ -31496,8 +31505,8 @@
       <c r="A80" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B80" s="3">
-        <v>44749</v>
+      <c r="B80" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>31</v>
@@ -31529,8 +31538,8 @@
       <c r="A81" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B81" s="3">
-        <v>44749</v>
+      <c r="B81" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>31</v>
@@ -31562,8 +31571,8 @@
       <c r="A82" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B82" s="3">
-        <v>44749</v>
+      <c r="B82" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>31</v>
@@ -31595,8 +31604,8 @@
       <c r="A83" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B83" s="3">
-        <v>44749</v>
+      <c r="B83" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>31</v>
@@ -31628,8 +31637,8 @@
       <c r="A84" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B84" s="3">
-        <v>44749</v>
+      <c r="B84" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>31</v>
@@ -31661,8 +31670,8 @@
       <c r="A85" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B85" s="3">
-        <v>44749</v>
+      <c r="B85" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>31</v>
@@ -31694,8 +31703,8 @@
       <c r="A86" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B86" s="3">
-        <v>44749</v>
+      <c r="B86" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>31</v>
@@ -31727,8 +31736,8 @@
       <c r="A87" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B87" s="3">
-        <v>44749</v>
+      <c r="B87" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>31</v>
@@ -31760,8 +31769,8 @@
       <c r="A88" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B88" s="3">
-        <v>44749</v>
+      <c r="B88" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>31</v>
@@ -31793,8 +31802,8 @@
       <c r="A89" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B89" s="3">
-        <v>44749</v>
+      <c r="B89" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>31</v>
@@ -31826,8 +31835,8 @@
       <c r="A90" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B90" s="3">
-        <v>44749</v>
+      <c r="B90" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>31</v>
@@ -31859,8 +31868,8 @@
       <c r="A91" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B91" s="3">
-        <v>44749</v>
+      <c r="B91" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>31</v>
@@ -31892,8 +31901,8 @@
       <c r="A92" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B92" s="3">
-        <v>44749</v>
+      <c r="B92" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>31</v>
@@ -31925,8 +31934,8 @@
       <c r="A93" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B93" s="3">
-        <v>44749</v>
+      <c r="B93" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>31</v>
@@ -31958,8 +31967,8 @@
       <c r="A94" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B94" s="3">
-        <v>44749</v>
+      <c r="B94" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>31</v>
@@ -31991,8 +32000,8 @@
       <c r="A95" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B95" s="3">
-        <v>44749</v>
+      <c r="B95" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>31</v>
@@ -32024,8 +32033,8 @@
       <c r="A96" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B96" s="3">
-        <v>44749</v>
+      <c r="B96" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>31</v>
@@ -32057,8 +32066,8 @@
       <c r="A97" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B97" s="3">
-        <v>44749</v>
+      <c r="B97" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>31</v>
@@ -32090,8 +32099,8 @@
       <c r="A98" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B98" s="3">
-        <v>44749</v>
+      <c r="B98" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>31</v>
@@ -32123,8 +32132,8 @@
       <c r="A99" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B99" s="3">
-        <v>44749</v>
+      <c r="B99" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>31</v>
@@ -32156,8 +32165,8 @@
       <c r="A100" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B100" s="3">
-        <v>44749</v>
+      <c r="B100" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>31</v>
@@ -32189,8 +32198,8 @@
       <c r="A101" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B101" s="3">
-        <v>44749</v>
+      <c r="B101" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>31</v>
@@ -32222,8 +32231,8 @@
       <c r="A102" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B102" s="3">
-        <v>44749</v>
+      <c r="B102" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>31</v>
@@ -32255,8 +32264,8 @@
       <c r="A103" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B103" s="3">
-        <v>44749</v>
+      <c r="B103" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>31</v>
@@ -32288,8 +32297,8 @@
       <c r="A104" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B104" s="3">
-        <v>44749</v>
+      <c r="B104" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>31</v>
@@ -32321,8 +32330,8 @@
       <c r="A105" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B105" s="3">
-        <v>44749</v>
+      <c r="B105" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>31</v>
@@ -32354,8 +32363,8 @@
       <c r="A106" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B106" s="3">
-        <v>44749</v>
+      <c r="B106" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>31</v>
@@ -32387,8 +32396,8 @@
       <c r="A107" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B107" s="3">
-        <v>44749</v>
+      <c r="B107" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>31</v>
@@ -32420,8 +32429,8 @@
       <c r="A108" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B108" s="3">
-        <v>44749</v>
+      <c r="B108" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>31</v>
@@ -32453,8 +32462,8 @@
       <c r="A109" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B109" s="3">
-        <v>44749</v>
+      <c r="B109" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>31</v>
@@ -32486,8 +32495,8 @@
       <c r="A110" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B110" s="3">
-        <v>44749</v>
+      <c r="B110" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>31</v>
@@ -32519,8 +32528,8 @@
       <c r="A111" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B111" s="3">
-        <v>44749</v>
+      <c r="B111" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>31</v>
@@ -32552,8 +32561,8 @@
       <c r="A112" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B112" s="3">
-        <v>44749</v>
+      <c r="B112" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>31</v>
@@ -32585,8 +32594,8 @@
       <c r="A113" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B113" s="3">
-        <v>44749</v>
+      <c r="B113" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>31</v>
@@ -32618,8 +32627,8 @@
       <c r="A114" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B114" s="3">
-        <v>44749</v>
+      <c r="B114" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>31</v>
@@ -32651,8 +32660,8 @@
       <c r="A115" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B115" s="3">
-        <v>44749</v>
+      <c r="B115" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>31</v>
@@ -32684,8 +32693,8 @@
       <c r="A116" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B116" s="3">
-        <v>44749</v>
+      <c r="B116" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>31</v>
@@ -32717,8 +32726,8 @@
       <c r="A117" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B117" s="3">
-        <v>44749</v>
+      <c r="B117" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>31</v>
@@ -32750,8 +32759,8 @@
       <c r="A118" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B118" s="3">
-        <v>44749</v>
+      <c r="B118" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>31</v>
@@ -32783,8 +32792,8 @@
       <c r="A119" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B119" s="3">
-        <v>44749</v>
+      <c r="B119" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>31</v>
@@ -32816,8 +32825,8 @@
       <c r="A120" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B120" s="3">
-        <v>44749</v>
+      <c r="B120" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>31</v>
@@ -32849,8 +32858,8 @@
       <c r="A121" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B121" s="3">
-        <v>44749</v>
+      <c r="B121" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>31</v>
@@ -32882,8 +32891,8 @@
       <c r="A122" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B122" s="3">
-        <v>44749</v>
+      <c r="B122" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>12</v>
@@ -32915,8 +32924,8 @@
       <c r="A123" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B123" s="3">
-        <v>44749</v>
+      <c r="B123" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>12</v>
@@ -32948,8 +32957,8 @@
       <c r="A124" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B124" s="3">
-        <v>44749</v>
+      <c r="B124" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>12</v>
@@ -32981,8 +32990,8 @@
       <c r="A125" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B125" s="3">
-        <v>44749</v>
+      <c r="B125" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>12</v>
@@ -33014,8 +33023,8 @@
       <c r="A126" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B126" s="3">
-        <v>44749</v>
+      <c r="B126" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>12</v>
@@ -33047,8 +33056,8 @@
       <c r="A127" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B127" s="3">
-        <v>44749</v>
+      <c r="B127" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>12</v>
@@ -33080,8 +33089,8 @@
       <c r="A128" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B128" s="3">
-        <v>44749</v>
+      <c r="B128" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>12</v>
@@ -33113,8 +33122,8 @@
       <c r="A129" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B129" s="3">
-        <v>44749</v>
+      <c r="B129" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>12</v>
@@ -33146,8 +33155,8 @@
       <c r="A130" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B130" s="3">
-        <v>44749</v>
+      <c r="B130" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>12</v>
@@ -33179,8 +33188,8 @@
       <c r="A131" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B131" s="3">
-        <v>44749</v>
+      <c r="B131" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>12</v>
@@ -33212,8 +33221,8 @@
       <c r="A132" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B132" s="3">
-        <v>44749</v>
+      <c r="B132" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>12</v>
@@ -33245,8 +33254,8 @@
       <c r="A133" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B133" s="3">
-        <v>44749</v>
+      <c r="B133" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>12</v>
@@ -33278,8 +33287,8 @@
       <c r="A134" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B134" s="3">
-        <v>44749</v>
+      <c r="B134" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>12</v>
@@ -33311,8 +33320,8 @@
       <c r="A135" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B135" s="3">
-        <v>44749</v>
+      <c r="B135" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>12</v>
@@ -33344,8 +33353,8 @@
       <c r="A136" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B136" s="3">
-        <v>44749</v>
+      <c r="B136" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>12</v>
@@ -33377,8 +33386,8 @@
       <c r="A137" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B137" s="3">
-        <v>44749</v>
+      <c r="B137" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>12</v>
@@ -33410,8 +33419,8 @@
       <c r="A138" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B138" s="3">
-        <v>44749</v>
+      <c r="B138" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>12</v>
@@ -33443,8 +33452,8 @@
       <c r="A139" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B139" s="3">
-        <v>44749</v>
+      <c r="B139" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>12</v>
@@ -33476,8 +33485,8 @@
       <c r="A140" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B140" s="3">
-        <v>44749</v>
+      <c r="B140" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>12</v>
@@ -33509,8 +33518,8 @@
       <c r="A141" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B141" s="3">
-        <v>44749</v>
+      <c r="B141" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>12</v>
@@ -33544,26 +33553,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="03c6cdc5-a326-4596-8bb5-5a108e6a189f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdb376e-ba08-4f94-9941-9e68dfd9ed35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D29CD47150B3D44192901CB20E6ABB56" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1b439f2d7c6d7abf5415dab7afed1a4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9bdb376e-ba08-4f94-9941-9e68dfd9ed35" xmlns:ns3="03c6cdc5-a326-4596-8bb5-5a108e6a189f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3257b63d3648651b426df57415bcf4c4" ns2:_="" ns3:_="">
     <xsd:import namespace="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
@@ -33752,10 +33741,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="03c6cdc5-a326-4596-8bb5-5a108e6a189f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdb376e-ba08-4f94-9941-9e68dfd9ed35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F20E8B07-673B-45FB-9B52-2C6DE9B56665}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937EA692-236A-4E27-A58D-20EAE7DF481C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
+    <ds:schemaRef ds:uri="03c6cdc5-a326-4596-8bb5-5a108e6a189f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -33772,20 +33792,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937EA692-236A-4E27-A58D-20EAE7DF481C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F20E8B07-673B-45FB-9B52-2C6DE9B56665}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
-    <ds:schemaRef ds:uri="03c6cdc5-a326-4596-8bb5-5a108e6a189f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add latest on mouse weights and proteomics
</commit_message>
<xml_diff>
--- a/DATA/body_weights_measurement.xlsx
+++ b/DATA/body_weights_measurement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgianaanderson/Documents/my_books/CODING-TEAM-BOOKDOWN-/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD3BDB2-263A-ED4E-BE87-54C956F91543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAAE3A4-40A9-9249-BC36-34AE1B036906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16180" activeTab="1" xr2:uid="{EF754327-75C9-0D46-A1B0-E47C524B8CAE}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16180" activeTab="6" xr2:uid="{EF754327-75C9-0D46-A1B0-E47C524B8CAE}"/>
   </bookViews>
   <sheets>
     <sheet name="before_vaccination" sheetId="1" r:id="rId1"/>
@@ -729,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC4A97D-A06C-3341-8FDE-C35378163F26}">
   <dimension ref="A1:L148"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A121" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
@@ -5381,8 +5381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C25201A-ED7D-4B98-B534-D23BB5ECFA5E}">
   <dimension ref="A1:L148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="131" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="A123" zoomScale="131" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8054,7 +8054,7 @@
         <v>3</v>
       </c>
       <c r="G80" s="1">
-        <v>2424</v>
+        <v>24.24</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>12</v>
@@ -10134,7 +10134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DEDDE3-1394-49BF-B818-8D3D8D78518B}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A120" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
@@ -14979,7 +14979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CEF4192-D164-4CF6-8C97-39E6CE474352}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A119" zoomScale="125" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
@@ -19804,7 +19804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E255660F-2462-47DD-A055-F25B5C708F02}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
+    <sheetView topLeftCell="A119" zoomScale="115" workbookViewId="0">
       <selection activeCell="I122" sqref="I122"/>
     </sheetView>
   </sheetViews>
@@ -24645,7 +24645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282F7039-F2FD-4D49-A7D4-099B758AE087}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A119" zoomScale="125" workbookViewId="0">
       <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
@@ -29509,8 +29509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF57C79E-F215-4103-AD42-D55276101BC9}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30126,7 +30126,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="12">
-        <v>2042</v>
+        <v>20.420000000000002</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>12</v>
@@ -34352,26 +34352,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="03c6cdc5-a326-4596-8bb5-5a108e6a189f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdb376e-ba08-4f94-9941-9e68dfd9ed35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D29CD47150B3D44192901CB20E6ABB56" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1b439f2d7c6d7abf5415dab7afed1a4a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9bdb376e-ba08-4f94-9941-9e68dfd9ed35" xmlns:ns3="03c6cdc5-a326-4596-8bb5-5a108e6a189f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3257b63d3648651b426df57415bcf4c4" ns2:_="" ns3:_="">
     <xsd:import namespace="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
@@ -34560,10 +34540,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="03c6cdc5-a326-4596-8bb5-5a108e6a189f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdb376e-ba08-4f94-9941-9e68dfd9ed35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F20E8B07-673B-45FB-9B52-2C6DE9B56665}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937EA692-236A-4E27-A58D-20EAE7DF481C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
+    <ds:schemaRef ds:uri="03c6cdc5-a326-4596-8bb5-5a108e6a189f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -34580,20 +34591,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937EA692-236A-4E27-A58D-20EAE7DF481C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F20E8B07-673B-45FB-9B52-2C6DE9B56665}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
-    <ds:schemaRef ds:uri="03c6cdc5-a326-4596-8bb5-5a108e6a189f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>